<commit_message>
Changes made in Readme
</commit_message>
<xml_diff>
--- a/MakeMyTrip_Group1_QEA21QE058.xlsx
+++ b/MakeMyTrip_Group1_QEA21QE058.xlsx
@@ -3,30 +3,34 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8824F36D-99B4-4D2F-BB71-B26103066CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prajw\eclipse-workspace\MMT_Booking_POM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517586FE-39A3-4631-A492-FAFC7AC6A724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="657" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Index" sheetId="5" r:id="rId1"/>
-    <sheet name="Requirement Analysis" sheetId="7" r:id="rId2"/>
-    <sheet name="TEST SCENARIO" sheetId="1" r:id="rId3"/>
-    <sheet name="Test Cases" sheetId="11" r:id="rId4"/>
-    <sheet name="SMOKE TESTCASE" sheetId="2" r:id="rId5"/>
-    <sheet name="REGRESSION TESTCASES" sheetId="6" r:id="rId6"/>
-    <sheet name="RTM" sheetId="4" r:id="rId7"/>
-    <sheet name="DEFECT REPORT" sheetId="3" r:id="rId8"/>
+    <sheet name="Requirement Analysis" sheetId="7" r:id="rId1"/>
+    <sheet name="TEST SCENARIO" sheetId="1" r:id="rId2"/>
+    <sheet name="Test Cases" sheetId="11" r:id="rId3"/>
+    <sheet name="SMOKE TESTCASE" sheetId="2" r:id="rId4"/>
+    <sheet name="REGRESSION TESTCASES" sheetId="6" r:id="rId5"/>
+    <sheet name="RTM" sheetId="4" r:id="rId6"/>
+    <sheet name="DEFECT REPORT" sheetId="3" r:id="rId7"/>
+    <sheet name="Index" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SMOKE TESTCASE'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SMOKE TESTCASE'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:K18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="250">
   <si>
     <t>Project ID</t>
   </si>
@@ -793,6 +797,9 @@
   </si>
   <si>
     <t xml:space="preserve">Prajwal Sabale </t>
+  </si>
+  <si>
+    <t>WebSite - https://www.makemytrip.com/</t>
   </si>
 </sst>
 </file>
@@ -1196,6 +1203,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1244,7 +1252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,311 +1555,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="31.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="77" t="s">
-        <v>248</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C8E961-5541-4E01-829A-46FF3D438A3C}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -1891,16 +1597,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="65">
+      <c r="A2" s="66">
         <v>1</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="62" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -1909,35 +1615,35 @@
       <c r="F2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="67" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="61"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="4" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="62"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="67"/>
+      <c r="G4" s="68"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E5" s="2"/>
@@ -1969,7 +1675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -2004,7 +1710,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="69" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -2021,7 +1727,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="69"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="22" t="s">
         <v>26</v>
       </c>
@@ -2036,7 +1742,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="22" t="s">
         <v>30</v>
       </c>
@@ -2051,7 +1757,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="69"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="22" t="s">
         <v>34</v>
       </c>
@@ -2066,7 +1772,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="69"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="22" t="s">
         <v>38</v>
       </c>
@@ -2081,7 +1787,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="70"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="24" t="s">
         <v>42</v>
       </c>
@@ -2136,7 +1842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0555AC-C749-4EB1-BFAA-F43C722EFA05}">
   <dimension ref="A1:K35"/>
   <sheetViews>
@@ -2197,7 +1903,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="72" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -2232,7 +1938,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="71"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="27" t="s">
         <v>67</v>
       </c>
@@ -2259,7 +1965,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="27" t="s">
         <v>73</v>
       </c>
@@ -2286,7 +1992,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="27" t="s">
         <v>78</v>
       </c>
@@ -2313,7 +2019,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="72" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -2342,7 +2048,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="71"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="27" t="s">
         <v>88</v>
       </c>
@@ -2369,7 +2075,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="27" t="s">
         <v>93</v>
       </c>
@@ -2399,7 +2105,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="27" t="s">
         <v>100</v>
       </c>
@@ -2426,7 +2132,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="71"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="27" t="s">
         <v>103</v>
       </c>
@@ -2456,7 +2162,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="27" t="s">
         <v>107</v>
       </c>
@@ -2483,7 +2189,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="27" t="s">
         <v>112</v>
       </c>
@@ -2513,7 +2219,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="27" t="s">
         <v>117</v>
       </c>
@@ -2540,7 +2246,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="27" t="s">
         <v>122</v>
       </c>
@@ -2567,7 +2273,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="27" t="s">
         <v>127</v>
       </c>
@@ -2597,7 +2303,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="27" t="s">
         <v>133</v>
       </c>
@@ -2624,7 +2330,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="74" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="27" t="s">
@@ -2653,7 +2359,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="73"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="27" t="s">
         <v>144</v>
       </c>
@@ -2680,7 +2386,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="73"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="27" t="s">
         <v>148</v>
       </c>
@@ -2707,7 +2413,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="73"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="27" t="s">
         <v>153</v>
       </c>
@@ -2737,7 +2443,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="73"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="27" t="s">
         <v>159</v>
       </c>
@@ -2764,7 +2470,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="72" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="27" t="s">
@@ -2793,7 +2499,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="71"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="27" t="s">
         <v>170</v>
       </c>
@@ -2820,7 +2526,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="71"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="27" t="s">
         <v>175</v>
       </c>
@@ -2847,7 +2553,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="72" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="27" t="s">
@@ -2876,7 +2582,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="71"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="27" t="s">
         <v>186</v>
       </c>
@@ -2906,7 +2612,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="71"/>
+      <c r="A27" s="72"/>
       <c r="B27" s="27" t="s">
         <v>192</v>
       </c>
@@ -2936,7 +2642,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="71"/>
+      <c r="A28" s="72"/>
       <c r="B28" s="27" t="s">
         <v>195</v>
       </c>
@@ -2966,7 +2672,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="71"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="27" t="s">
         <v>198</v>
       </c>
@@ -2996,7 +2702,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="71"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="27" t="s">
         <v>203</v>
       </c>
@@ -3026,7 +2732,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="72" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="27" t="s">
@@ -3055,7 +2761,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="71"/>
+      <c r="A32" s="72"/>
       <c r="B32" s="27" t="s">
         <v>213</v>
       </c>
@@ -3082,7 +2788,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="72"/>
+      <c r="A33" s="73"/>
       <c r="B33" s="35" t="s">
         <v>217</v>
       </c>
@@ -3113,7 +2819,7 @@
     <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:11" ht="15.45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
     </row>
   </sheetData>
@@ -3131,7 +2837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -3189,7 +2895,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="72" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="39" t="s">
@@ -3217,7 +2923,7 @@
       <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="71"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="39" t="s">
         <v>67</v>
       </c>
@@ -3243,7 +2949,7 @@
       <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="39" t="s">
         <v>73</v>
       </c>
@@ -3269,7 +2975,7 @@
       <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="39" t="s">
         <v>78</v>
       </c>
@@ -3295,7 +3001,7 @@
       <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="39" t="s">
@@ -3322,7 +3028,7 @@
       <c r="J6" s="45"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="75"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="39" t="s">
         <v>88</v>
       </c>
@@ -3347,7 +3053,7 @@
       <c r="J7" s="45"/>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
+      <c r="A8" s="76"/>
       <c r="B8" s="39" t="s">
         <v>100</v>
       </c>
@@ -3372,7 +3078,7 @@
       <c r="J8" s="45"/>
     </row>
     <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="75"/>
+      <c r="A9" s="76"/>
       <c r="B9" s="39" t="s">
         <v>107</v>
       </c>
@@ -3397,7 +3103,7 @@
       <c r="J9" s="45"/>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="75"/>
+      <c r="A10" s="76"/>
       <c r="B10" s="39" t="s">
         <v>117</v>
       </c>
@@ -3422,7 +3128,7 @@
       <c r="J10" s="45"/>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="75"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="39" t="s">
         <v>122</v>
       </c>
@@ -3447,7 +3153,7 @@
       <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="76" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="39" t="s">
@@ -3474,7 +3180,7 @@
       <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="75"/>
+      <c r="A13" s="76"/>
       <c r="B13" s="39" t="s">
         <v>148</v>
       </c>
@@ -3499,7 +3205,7 @@
       <c r="J13" s="45"/>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="75" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="39" t="s">
@@ -3526,7 +3232,7 @@
       <c r="J14" s="45"/>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="74"/>
+      <c r="A15" s="75"/>
       <c r="B15" s="39" t="s">
         <v>170</v>
       </c>
@@ -3551,7 +3257,7 @@
       <c r="J15" s="45"/>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="74"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="39" t="s">
         <v>175</v>
       </c>
@@ -3603,7 +3309,7 @@
       <c r="J17" s="45"/>
     </row>
     <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="76" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="39" t="s">
@@ -3629,8 +3335,8 @@
       </c>
       <c r="J18" s="45"/>
     </row>
-    <row r="19" spans="1:10" ht="28.95" x14ac:dyDescent="0.35">
-      <c r="A19" s="76"/>
+    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="77"/>
       <c r="B19" s="47" t="s">
         <v>213</v>
       </c>
@@ -3669,7 +3375,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2319C3-7CFD-4DC1-87DF-2910E50A345A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -3725,7 +3431,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="39" t="s">
@@ -3752,7 +3458,7 @@
       <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="75"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="39" t="s">
         <v>103</v>
       </c>
@@ -3777,7 +3483,7 @@
       <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="39" t="s">
         <v>112</v>
       </c>
@@ -3802,7 +3508,7 @@
       <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="75"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="39" t="s">
         <v>127</v>
       </c>
@@ -3827,7 +3533,7 @@
       <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="75"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="39" t="s">
         <v>133</v>
       </c>
@@ -3852,7 +3558,7 @@
       <c r="J6" s="45"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="76" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="39" t="s">
@@ -3879,7 +3585,7 @@
       <c r="J7" s="45"/>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
+      <c r="A8" s="76"/>
       <c r="B8" s="39" t="s">
         <v>153</v>
       </c>
@@ -3904,7 +3610,7 @@
       <c r="J8" s="45"/>
     </row>
     <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="75"/>
+      <c r="A9" s="76"/>
       <c r="B9" s="39" t="s">
         <v>159</v>
       </c>
@@ -3929,7 +3635,7 @@
       <c r="J9" s="45"/>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="76" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="39" t="s">
@@ -3956,7 +3662,7 @@
       <c r="J10" s="45"/>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="75"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="39" t="s">
         <v>192</v>
       </c>
@@ -3981,7 +3687,7 @@
       <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="75"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="39" t="s">
         <v>195</v>
       </c>
@@ -4006,7 +3712,7 @@
       <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="75"/>
+      <c r="A13" s="76"/>
       <c r="B13" s="39" t="s">
         <v>198</v>
       </c>
@@ -4031,7 +3737,7 @@
       <c r="J13" s="45"/>
     </row>
     <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="75"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="39" t="s">
         <v>203</v>
       </c>
@@ -4095,7 +3801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -4247,7 +3953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -4318,4 +4024,307 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="31.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="61" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>